<commit_message>
Added back soles and trinys
</commit_message>
<xml_diff>
--- a/PurchaseOrder_Scheduler/schedule_insert_spreadsheet.xlsx
+++ b/PurchaseOrder_Scheduler/schedule_insert_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipe\Documents\purchase_planner\PurchaseOrder_Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BB1F3B1A-DA9D-4CF1-8ACA-DCD00740538B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0C803FF-9FE7-4CC9-9656-22128F4D11BC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="25">
   <si>
     <t>vendor_name</t>
   </si>
@@ -539,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D251"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="H211" sqref="H211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3543,6 +3543,744 @@
         <v>43441</v>
       </c>
       <c r="D201" s="1">
+        <v>43490</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>5</v>
+      </c>
+      <c r="B202">
+        <v>68</v>
+      </c>
+      <c r="C202" s="1">
+        <v>43070</v>
+      </c>
+      <c r="D202" s="1">
+        <v>43119</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>5</v>
+      </c>
+      <c r="B203">
+        <v>68</v>
+      </c>
+      <c r="C203" s="1">
+        <v>43084</v>
+      </c>
+      <c r="D203" s="1">
+        <v>43133</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>5</v>
+      </c>
+      <c r="B204">
+        <v>68</v>
+      </c>
+      <c r="C204" s="1">
+        <v>43119</v>
+      </c>
+      <c r="D204" s="1">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>5</v>
+      </c>
+      <c r="B205">
+        <v>68</v>
+      </c>
+      <c r="C205" s="1">
+        <v>43133</v>
+      </c>
+      <c r="D205" s="1">
+        <v>43161</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>5</v>
+      </c>
+      <c r="B206">
+        <v>68</v>
+      </c>
+      <c r="C206" s="1">
+        <v>43147</v>
+      </c>
+      <c r="D206" s="1">
+        <f t="shared" ref="D206:D224" si="0">C208</f>
+        <v>43175</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>5</v>
+      </c>
+      <c r="B207">
+        <v>68</v>
+      </c>
+      <c r="C207" s="1">
+        <v>43161</v>
+      </c>
+      <c r="D207" s="1">
+        <f t="shared" si="0"/>
+        <v>43189</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>5</v>
+      </c>
+      <c r="B208">
+        <v>68</v>
+      </c>
+      <c r="C208" s="1">
+        <v>43175</v>
+      </c>
+      <c r="D208" s="1">
+        <f t="shared" si="0"/>
+        <v>43203</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>5</v>
+      </c>
+      <c r="B209">
+        <v>68</v>
+      </c>
+      <c r="C209" s="1">
+        <v>43189</v>
+      </c>
+      <c r="D209" s="1">
+        <f t="shared" si="0"/>
+        <v>43217</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>5</v>
+      </c>
+      <c r="B210">
+        <v>68</v>
+      </c>
+      <c r="C210" s="1">
+        <v>43203</v>
+      </c>
+      <c r="D210" s="1">
+        <f t="shared" si="0"/>
+        <v>43231</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>5</v>
+      </c>
+      <c r="B211">
+        <v>68</v>
+      </c>
+      <c r="C211" s="1">
+        <v>43217</v>
+      </c>
+      <c r="D211" s="1">
+        <f t="shared" si="0"/>
+        <v>43245</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>5</v>
+      </c>
+      <c r="B212">
+        <v>68</v>
+      </c>
+      <c r="C212" s="1">
+        <v>43231</v>
+      </c>
+      <c r="D212" s="1">
+        <f t="shared" si="0"/>
+        <v>43259</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>5</v>
+      </c>
+      <c r="B213">
+        <v>68</v>
+      </c>
+      <c r="C213" s="1">
+        <v>43245</v>
+      </c>
+      <c r="D213" s="1">
+        <f t="shared" si="0"/>
+        <v>43273</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>5</v>
+      </c>
+      <c r="B214">
+        <v>68</v>
+      </c>
+      <c r="C214" s="1">
+        <v>43259</v>
+      </c>
+      <c r="D214" s="1">
+        <f t="shared" si="0"/>
+        <v>43271</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>5</v>
+      </c>
+      <c r="B215">
+        <v>68</v>
+      </c>
+      <c r="C215" s="1">
+        <v>43273</v>
+      </c>
+      <c r="D215" s="1">
+        <f t="shared" si="0"/>
+        <v>43315</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>5</v>
+      </c>
+      <c r="B216">
+        <v>68</v>
+      </c>
+      <c r="C216" s="1">
+        <v>43271</v>
+      </c>
+      <c r="D216" s="1">
+        <f t="shared" si="0"/>
+        <v>43329</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>5</v>
+      </c>
+      <c r="B217">
+        <v>68</v>
+      </c>
+      <c r="C217" s="1">
+        <v>43315</v>
+      </c>
+      <c r="D217" s="1">
+        <f t="shared" si="0"/>
+        <v>43343</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>5</v>
+      </c>
+      <c r="B218">
+        <v>68</v>
+      </c>
+      <c r="C218" s="1">
+        <v>43329</v>
+      </c>
+      <c r="D218" s="1">
+        <f t="shared" si="0"/>
+        <v>43357</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>5</v>
+      </c>
+      <c r="B219">
+        <v>68</v>
+      </c>
+      <c r="C219" s="1">
+        <v>43343</v>
+      </c>
+      <c r="D219" s="1">
+        <f t="shared" si="0"/>
+        <v>43371</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>5</v>
+      </c>
+      <c r="B220">
+        <v>68</v>
+      </c>
+      <c r="C220" s="1">
+        <v>43357</v>
+      </c>
+      <c r="D220" s="1">
+        <f t="shared" si="0"/>
+        <v>43385</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>5</v>
+      </c>
+      <c r="B221">
+        <v>68</v>
+      </c>
+      <c r="C221" s="1">
+        <v>43371</v>
+      </c>
+      <c r="D221" s="1">
+        <f t="shared" si="0"/>
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>5</v>
+      </c>
+      <c r="B222">
+        <v>68</v>
+      </c>
+      <c r="C222" s="1">
+        <v>43385</v>
+      </c>
+      <c r="D222" s="1">
+        <f t="shared" si="0"/>
+        <v>43413</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>5</v>
+      </c>
+      <c r="B223">
+        <v>68</v>
+      </c>
+      <c r="C223" s="1">
+        <v>43399</v>
+      </c>
+      <c r="D223" s="1">
+        <f t="shared" si="0"/>
+        <v>43427</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>5</v>
+      </c>
+      <c r="B224">
+        <v>68</v>
+      </c>
+      <c r="C224" s="1">
+        <v>43413</v>
+      </c>
+      <c r="D224" s="1">
+        <f t="shared" si="0"/>
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>5</v>
+      </c>
+      <c r="B225">
+        <v>68</v>
+      </c>
+      <c r="C225" s="1">
+        <v>43427</v>
+      </c>
+      <c r="D225" s="1">
+        <v>43455</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>5</v>
+      </c>
+      <c r="B226">
+        <v>68</v>
+      </c>
+      <c r="C226" s="1">
+        <v>43441</v>
+      </c>
+      <c r="D226" s="1">
+        <v>43490</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>4</v>
+      </c>
+      <c r="B227">
+        <v>69</v>
+      </c>
+      <c r="C227" s="1">
+        <v>43070</v>
+      </c>
+      <c r="D227" s="1">
+        <v>43119</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>4</v>
+      </c>
+      <c r="B228">
+        <v>69</v>
+      </c>
+      <c r="C228" s="1">
+        <v>43084</v>
+      </c>
+      <c r="D228" s="1">
+        <v>43133</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>4</v>
+      </c>
+      <c r="B229">
+        <v>69</v>
+      </c>
+      <c r="C229" s="1">
+        <v>43119</v>
+      </c>
+      <c r="D229" s="1">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>4</v>
+      </c>
+      <c r="B230">
+        <v>69</v>
+      </c>
+      <c r="C230" s="1">
+        <v>43133</v>
+      </c>
+      <c r="D230" s="1">
+        <v>43161</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>4</v>
+      </c>
+      <c r="B231">
+        <v>69</v>
+      </c>
+      <c r="C231" s="1">
+        <v>43147</v>
+      </c>
+      <c r="D231" s="1">
+        <f t="shared" ref="D231:D249" si="1">C233</f>
+        <v>43175</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>4</v>
+      </c>
+      <c r="B232">
+        <v>69</v>
+      </c>
+      <c r="C232" s="1">
+        <v>43161</v>
+      </c>
+      <c r="D232" s="1">
+        <f t="shared" si="1"/>
+        <v>43189</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>4</v>
+      </c>
+      <c r="B233">
+        <v>69</v>
+      </c>
+      <c r="C233" s="1">
+        <v>43175</v>
+      </c>
+      <c r="D233" s="1">
+        <f t="shared" si="1"/>
+        <v>43203</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>4</v>
+      </c>
+      <c r="B234">
+        <v>69</v>
+      </c>
+      <c r="C234" s="1">
+        <v>43189</v>
+      </c>
+      <c r="D234" s="1">
+        <f t="shared" si="1"/>
+        <v>43217</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>4</v>
+      </c>
+      <c r="B235">
+        <v>69</v>
+      </c>
+      <c r="C235" s="1">
+        <v>43203</v>
+      </c>
+      <c r="D235" s="1">
+        <f t="shared" si="1"/>
+        <v>43231</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>4</v>
+      </c>
+      <c r="B236">
+        <v>69</v>
+      </c>
+      <c r="C236" s="1">
+        <v>43217</v>
+      </c>
+      <c r="D236" s="1">
+        <f t="shared" si="1"/>
+        <v>43245</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>4</v>
+      </c>
+      <c r="B237">
+        <v>69</v>
+      </c>
+      <c r="C237" s="1">
+        <v>43231</v>
+      </c>
+      <c r="D237" s="1">
+        <f t="shared" si="1"/>
+        <v>43259</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>4</v>
+      </c>
+      <c r="B238">
+        <v>69</v>
+      </c>
+      <c r="C238" s="1">
+        <v>43245</v>
+      </c>
+      <c r="D238" s="1">
+        <f t="shared" si="1"/>
+        <v>43273</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>4</v>
+      </c>
+      <c r="B239">
+        <v>69</v>
+      </c>
+      <c r="C239" s="1">
+        <v>43259</v>
+      </c>
+      <c r="D239" s="1">
+        <f t="shared" si="1"/>
+        <v>43271</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>4</v>
+      </c>
+      <c r="B240">
+        <v>69</v>
+      </c>
+      <c r="C240" s="1">
+        <v>43273</v>
+      </c>
+      <c r="D240" s="1">
+        <f t="shared" si="1"/>
+        <v>43315</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>4</v>
+      </c>
+      <c r="B241">
+        <v>69</v>
+      </c>
+      <c r="C241" s="1">
+        <v>43271</v>
+      </c>
+      <c r="D241" s="1">
+        <f t="shared" si="1"/>
+        <v>43329</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>4</v>
+      </c>
+      <c r="B242">
+        <v>69</v>
+      </c>
+      <c r="C242" s="1">
+        <v>43315</v>
+      </c>
+      <c r="D242" s="1">
+        <f t="shared" si="1"/>
+        <v>43343</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>4</v>
+      </c>
+      <c r="B243">
+        <v>69</v>
+      </c>
+      <c r="C243" s="1">
+        <v>43329</v>
+      </c>
+      <c r="D243" s="1">
+        <f t="shared" si="1"/>
+        <v>43357</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>4</v>
+      </c>
+      <c r="B244">
+        <v>69</v>
+      </c>
+      <c r="C244" s="1">
+        <v>43343</v>
+      </c>
+      <c r="D244" s="1">
+        <f t="shared" si="1"/>
+        <v>43371</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>4</v>
+      </c>
+      <c r="B245">
+        <v>69</v>
+      </c>
+      <c r="C245" s="1">
+        <v>43357</v>
+      </c>
+      <c r="D245" s="1">
+        <f t="shared" si="1"/>
+        <v>43385</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>4</v>
+      </c>
+      <c r="B246">
+        <v>69</v>
+      </c>
+      <c r="C246" s="1">
+        <v>43371</v>
+      </c>
+      <c r="D246" s="1">
+        <f t="shared" si="1"/>
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>4</v>
+      </c>
+      <c r="B247">
+        <v>69</v>
+      </c>
+      <c r="C247" s="1">
+        <v>43385</v>
+      </c>
+      <c r="D247" s="1">
+        <f t="shared" si="1"/>
+        <v>43413</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>4</v>
+      </c>
+      <c r="B248">
+        <v>69</v>
+      </c>
+      <c r="C248" s="1">
+        <v>43399</v>
+      </c>
+      <c r="D248" s="1">
+        <f t="shared" si="1"/>
+        <v>43427</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>4</v>
+      </c>
+      <c r="B249">
+        <v>69</v>
+      </c>
+      <c r="C249" s="1">
+        <v>43413</v>
+      </c>
+      <c r="D249" s="1">
+        <f t="shared" si="1"/>
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>4</v>
+      </c>
+      <c r="B250">
+        <v>69</v>
+      </c>
+      <c r="C250" s="1">
+        <v>43427</v>
+      </c>
+      <c r="D250" s="1">
+        <v>43455</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>4</v>
+      </c>
+      <c r="B251">
+        <v>69</v>
+      </c>
+      <c r="C251" s="1">
+        <v>43441</v>
+      </c>
+      <c r="D251" s="1">
         <v>43490</v>
       </c>
     </row>
@@ -3562,10 +4300,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I236"/>
+  <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="A262" sqref="A262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10181,112 +10919,1654 @@
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H201" s="3"/>
+      <c r="A201" t="s">
+        <v>9</v>
+      </c>
+      <c r="B201" t="str">
+        <f>schedule!A202</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C201" t="s">
+        <v>10</v>
+      </c>
+      <c r="D201">
+        <f>schedule!B202</f>
+        <v>68</v>
+      </c>
+      <c r="E201" t="s">
+        <v>11</v>
+      </c>
+      <c r="F201" s="2">
+        <f>schedule!C202</f>
+        <v>43070</v>
+      </c>
+      <c r="G201" t="s">
+        <v>12</v>
+      </c>
+      <c r="H201" s="3">
+        <f>schedule!D202</f>
+        <v>43119</v>
+      </c>
+      <c r="I201" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H202" s="3"/>
+      <c r="A202" t="s">
+        <v>9</v>
+      </c>
+      <c r="B202" t="str">
+        <f>schedule!A203</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C202" t="s">
+        <v>10</v>
+      </c>
+      <c r="D202">
+        <f>schedule!B203</f>
+        <v>68</v>
+      </c>
+      <c r="E202" t="s">
+        <v>11</v>
+      </c>
+      <c r="F202" s="2">
+        <f>schedule!C203</f>
+        <v>43084</v>
+      </c>
+      <c r="G202" t="s">
+        <v>12</v>
+      </c>
+      <c r="H202" s="3">
+        <f>schedule!D203</f>
+        <v>43133</v>
+      </c>
+      <c r="I202" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H203" s="3"/>
+      <c r="A203" t="s">
+        <v>9</v>
+      </c>
+      <c r="B203" t="str">
+        <f>schedule!A204</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C203" t="s">
+        <v>10</v>
+      </c>
+      <c r="D203">
+        <f>schedule!B204</f>
+        <v>68</v>
+      </c>
+      <c r="E203" t="s">
+        <v>11</v>
+      </c>
+      <c r="F203" s="2">
+        <f>schedule!C204</f>
+        <v>43119</v>
+      </c>
+      <c r="G203" t="s">
+        <v>12</v>
+      </c>
+      <c r="H203" s="3">
+        <f>schedule!D204</f>
+        <v>43147</v>
+      </c>
+      <c r="I203" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H204" s="3"/>
+      <c r="A204" t="s">
+        <v>9</v>
+      </c>
+      <c r="B204" t="str">
+        <f>schedule!A205</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C204" t="s">
+        <v>10</v>
+      </c>
+      <c r="D204">
+        <f>schedule!B205</f>
+        <v>68</v>
+      </c>
+      <c r="E204" t="s">
+        <v>11</v>
+      </c>
+      <c r="F204" s="2">
+        <f>schedule!C205</f>
+        <v>43133</v>
+      </c>
+      <c r="G204" t="s">
+        <v>12</v>
+      </c>
+      <c r="H204" s="3">
+        <f>schedule!D205</f>
+        <v>43161</v>
+      </c>
+      <c r="I204" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H205" s="3"/>
+      <c r="A205" t="s">
+        <v>9</v>
+      </c>
+      <c r="B205" t="str">
+        <f>schedule!A206</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C205" t="s">
+        <v>10</v>
+      </c>
+      <c r="D205">
+        <f>schedule!B206</f>
+        <v>68</v>
+      </c>
+      <c r="E205" t="s">
+        <v>11</v>
+      </c>
+      <c r="F205" s="2">
+        <f>schedule!C206</f>
+        <v>43147</v>
+      </c>
+      <c r="G205" t="s">
+        <v>12</v>
+      </c>
+      <c r="H205" s="3">
+        <f>schedule!D206</f>
+        <v>43175</v>
+      </c>
+      <c r="I205" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H206" s="3"/>
+      <c r="A206" t="s">
+        <v>9</v>
+      </c>
+      <c r="B206" t="str">
+        <f>schedule!A207</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C206" t="s">
+        <v>10</v>
+      </c>
+      <c r="D206">
+        <f>schedule!B207</f>
+        <v>68</v>
+      </c>
+      <c r="E206" t="s">
+        <v>11</v>
+      </c>
+      <c r="F206" s="2">
+        <f>schedule!C207</f>
+        <v>43161</v>
+      </c>
+      <c r="G206" t="s">
+        <v>12</v>
+      </c>
+      <c r="H206" s="3">
+        <f>schedule!D207</f>
+        <v>43189</v>
+      </c>
+      <c r="I206" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H207" s="3"/>
+      <c r="A207" t="s">
+        <v>9</v>
+      </c>
+      <c r="B207" t="str">
+        <f>schedule!A208</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C207" t="s">
+        <v>10</v>
+      </c>
+      <c r="D207">
+        <f>schedule!B208</f>
+        <v>68</v>
+      </c>
+      <c r="E207" t="s">
+        <v>11</v>
+      </c>
+      <c r="F207" s="2">
+        <f>schedule!C208</f>
+        <v>43175</v>
+      </c>
+      <c r="G207" t="s">
+        <v>12</v>
+      </c>
+      <c r="H207" s="3">
+        <f>schedule!D208</f>
+        <v>43203</v>
+      </c>
+      <c r="I207" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H208" s="3"/>
-    </row>
-    <row r="209" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H209" s="3"/>
-    </row>
-    <row r="210" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H210" s="3"/>
-    </row>
-    <row r="211" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H211" s="3"/>
-    </row>
-    <row r="212" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H212" s="3"/>
-    </row>
-    <row r="213" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H213" s="3"/>
-    </row>
-    <row r="214" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H214" s="3"/>
-    </row>
-    <row r="215" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H215" s="3"/>
-    </row>
-    <row r="216" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H216" s="3"/>
-    </row>
-    <row r="217" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H217" s="3"/>
-    </row>
-    <row r="218" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H218" s="3"/>
-    </row>
-    <row r="219" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H219" s="3"/>
-    </row>
-    <row r="220" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H220" s="3"/>
-    </row>
-    <row r="221" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H221" s="3"/>
-    </row>
-    <row r="222" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H222" s="3"/>
-    </row>
-    <row r="223" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H223" s="3"/>
-    </row>
-    <row r="224" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H224" s="3"/>
-    </row>
-    <row r="225" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H225" s="3"/>
-    </row>
-    <row r="226" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H226" s="3"/>
-    </row>
-    <row r="227" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H227" s="3"/>
-    </row>
-    <row r="228" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H228" s="3"/>
-    </row>
-    <row r="229" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H229" s="3"/>
-    </row>
-    <row r="230" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H230" s="3"/>
-    </row>
-    <row r="231" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H231" s="3"/>
-    </row>
-    <row r="232" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H232" s="3"/>
-    </row>
-    <row r="233" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H233" s="3"/>
-    </row>
-    <row r="234" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H234" s="3"/>
-    </row>
-    <row r="235" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H235" s="3"/>
-    </row>
-    <row r="236" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H236" s="3"/>
+      <c r="A208" t="s">
+        <v>9</v>
+      </c>
+      <c r="B208" t="str">
+        <f>schedule!A209</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C208" t="s">
+        <v>10</v>
+      </c>
+      <c r="D208">
+        <f>schedule!B209</f>
+        <v>68</v>
+      </c>
+      <c r="E208" t="s">
+        <v>11</v>
+      </c>
+      <c r="F208" s="2">
+        <f>schedule!C209</f>
+        <v>43189</v>
+      </c>
+      <c r="G208" t="s">
+        <v>12</v>
+      </c>
+      <c r="H208" s="3">
+        <f>schedule!D209</f>
+        <v>43217</v>
+      </c>
+      <c r="I208" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>9</v>
+      </c>
+      <c r="B209" t="str">
+        <f>schedule!A210</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C209" t="s">
+        <v>10</v>
+      </c>
+      <c r="D209">
+        <f>schedule!B210</f>
+        <v>68</v>
+      </c>
+      <c r="E209" t="s">
+        <v>11</v>
+      </c>
+      <c r="F209" s="2">
+        <f>schedule!C210</f>
+        <v>43203</v>
+      </c>
+      <c r="G209" t="s">
+        <v>12</v>
+      </c>
+      <c r="H209" s="3">
+        <f>schedule!D210</f>
+        <v>43231</v>
+      </c>
+      <c r="I209" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>9</v>
+      </c>
+      <c r="B210" t="str">
+        <f>schedule!A211</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C210" t="s">
+        <v>10</v>
+      </c>
+      <c r="D210">
+        <f>schedule!B211</f>
+        <v>68</v>
+      </c>
+      <c r="E210" t="s">
+        <v>11</v>
+      </c>
+      <c r="F210" s="2">
+        <f>schedule!C211</f>
+        <v>43217</v>
+      </c>
+      <c r="G210" t="s">
+        <v>12</v>
+      </c>
+      <c r="H210" s="3">
+        <f>schedule!D211</f>
+        <v>43245</v>
+      </c>
+      <c r="I210" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>9</v>
+      </c>
+      <c r="B211" t="str">
+        <f>schedule!A212</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C211" t="s">
+        <v>10</v>
+      </c>
+      <c r="D211">
+        <f>schedule!B212</f>
+        <v>68</v>
+      </c>
+      <c r="E211" t="s">
+        <v>11</v>
+      </c>
+      <c r="F211" s="2">
+        <f>schedule!C212</f>
+        <v>43231</v>
+      </c>
+      <c r="G211" t="s">
+        <v>12</v>
+      </c>
+      <c r="H211" s="3">
+        <f>schedule!D212</f>
+        <v>43259</v>
+      </c>
+      <c r="I211" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>9</v>
+      </c>
+      <c r="B212" t="str">
+        <f>schedule!A213</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C212" t="s">
+        <v>10</v>
+      </c>
+      <c r="D212">
+        <f>schedule!B213</f>
+        <v>68</v>
+      </c>
+      <c r="E212" t="s">
+        <v>11</v>
+      </c>
+      <c r="F212" s="2">
+        <f>schedule!C213</f>
+        <v>43245</v>
+      </c>
+      <c r="G212" t="s">
+        <v>12</v>
+      </c>
+      <c r="H212" s="3">
+        <f>schedule!D213</f>
+        <v>43273</v>
+      </c>
+      <c r="I212" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>9</v>
+      </c>
+      <c r="B213" t="str">
+        <f>schedule!A214</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C213" t="s">
+        <v>10</v>
+      </c>
+      <c r="D213">
+        <f>schedule!B214</f>
+        <v>68</v>
+      </c>
+      <c r="E213" t="s">
+        <v>11</v>
+      </c>
+      <c r="F213" s="2">
+        <f>schedule!C214</f>
+        <v>43259</v>
+      </c>
+      <c r="G213" t="s">
+        <v>12</v>
+      </c>
+      <c r="H213" s="3">
+        <f>schedule!D214</f>
+        <v>43271</v>
+      </c>
+      <c r="I213" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>9</v>
+      </c>
+      <c r="B214" t="str">
+        <f>schedule!A215</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C214" t="s">
+        <v>10</v>
+      </c>
+      <c r="D214">
+        <f>schedule!B215</f>
+        <v>68</v>
+      </c>
+      <c r="E214" t="s">
+        <v>11</v>
+      </c>
+      <c r="F214" s="2">
+        <f>schedule!C215</f>
+        <v>43273</v>
+      </c>
+      <c r="G214" t="s">
+        <v>12</v>
+      </c>
+      <c r="H214" s="3">
+        <f>schedule!D215</f>
+        <v>43315</v>
+      </c>
+      <c r="I214" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>9</v>
+      </c>
+      <c r="B215" t="str">
+        <f>schedule!A216</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C215" t="s">
+        <v>10</v>
+      </c>
+      <c r="D215">
+        <f>schedule!B216</f>
+        <v>68</v>
+      </c>
+      <c r="E215" t="s">
+        <v>11</v>
+      </c>
+      <c r="F215" s="2">
+        <f>schedule!C216</f>
+        <v>43271</v>
+      </c>
+      <c r="G215" t="s">
+        <v>12</v>
+      </c>
+      <c r="H215" s="3">
+        <f>schedule!D216</f>
+        <v>43329</v>
+      </c>
+      <c r="I215" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>9</v>
+      </c>
+      <c r="B216" t="str">
+        <f>schedule!A217</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C216" t="s">
+        <v>10</v>
+      </c>
+      <c r="D216">
+        <f>schedule!B217</f>
+        <v>68</v>
+      </c>
+      <c r="E216" t="s">
+        <v>11</v>
+      </c>
+      <c r="F216" s="2">
+        <f>schedule!C217</f>
+        <v>43315</v>
+      </c>
+      <c r="G216" t="s">
+        <v>12</v>
+      </c>
+      <c r="H216" s="3">
+        <f>schedule!D217</f>
+        <v>43343</v>
+      </c>
+      <c r="I216" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>9</v>
+      </c>
+      <c r="B217" t="str">
+        <f>schedule!A218</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C217" t="s">
+        <v>10</v>
+      </c>
+      <c r="D217">
+        <f>schedule!B218</f>
+        <v>68</v>
+      </c>
+      <c r="E217" t="s">
+        <v>11</v>
+      </c>
+      <c r="F217" s="2">
+        <f>schedule!C218</f>
+        <v>43329</v>
+      </c>
+      <c r="G217" t="s">
+        <v>12</v>
+      </c>
+      <c r="H217" s="3">
+        <f>schedule!D218</f>
+        <v>43357</v>
+      </c>
+      <c r="I217" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>9</v>
+      </c>
+      <c r="B218" t="str">
+        <f>schedule!A219</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C218" t="s">
+        <v>10</v>
+      </c>
+      <c r="D218">
+        <f>schedule!B219</f>
+        <v>68</v>
+      </c>
+      <c r="E218" t="s">
+        <v>11</v>
+      </c>
+      <c r="F218" s="2">
+        <f>schedule!C219</f>
+        <v>43343</v>
+      </c>
+      <c r="G218" t="s">
+        <v>12</v>
+      </c>
+      <c r="H218" s="3">
+        <f>schedule!D219</f>
+        <v>43371</v>
+      </c>
+      <c r="I218" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>9</v>
+      </c>
+      <c r="B219" t="str">
+        <f>schedule!A220</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C219" t="s">
+        <v>10</v>
+      </c>
+      <c r="D219">
+        <f>schedule!B220</f>
+        <v>68</v>
+      </c>
+      <c r="E219" t="s">
+        <v>11</v>
+      </c>
+      <c r="F219" s="2">
+        <f>schedule!C220</f>
+        <v>43357</v>
+      </c>
+      <c r="G219" t="s">
+        <v>12</v>
+      </c>
+      <c r="H219" s="3">
+        <f>schedule!D220</f>
+        <v>43385</v>
+      </c>
+      <c r="I219" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>9</v>
+      </c>
+      <c r="B220" t="str">
+        <f>schedule!A221</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C220" t="s">
+        <v>10</v>
+      </c>
+      <c r="D220">
+        <f>schedule!B221</f>
+        <v>68</v>
+      </c>
+      <c r="E220" t="s">
+        <v>11</v>
+      </c>
+      <c r="F220" s="2">
+        <f>schedule!C221</f>
+        <v>43371</v>
+      </c>
+      <c r="G220" t="s">
+        <v>12</v>
+      </c>
+      <c r="H220" s="3">
+        <f>schedule!D221</f>
+        <v>43399</v>
+      </c>
+      <c r="I220" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>9</v>
+      </c>
+      <c r="B221" t="str">
+        <f>schedule!A222</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C221" t="s">
+        <v>10</v>
+      </c>
+      <c r="D221">
+        <f>schedule!B222</f>
+        <v>68</v>
+      </c>
+      <c r="E221" t="s">
+        <v>11</v>
+      </c>
+      <c r="F221" s="2">
+        <f>schedule!C222</f>
+        <v>43385</v>
+      </c>
+      <c r="G221" t="s">
+        <v>12</v>
+      </c>
+      <c r="H221" s="3">
+        <f>schedule!D222</f>
+        <v>43413</v>
+      </c>
+      <c r="I221" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>9</v>
+      </c>
+      <c r="B222" t="str">
+        <f>schedule!A223</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C222" t="s">
+        <v>10</v>
+      </c>
+      <c r="D222">
+        <f>schedule!B223</f>
+        <v>68</v>
+      </c>
+      <c r="E222" t="s">
+        <v>11</v>
+      </c>
+      <c r="F222" s="2">
+        <f>schedule!C223</f>
+        <v>43399</v>
+      </c>
+      <c r="G222" t="s">
+        <v>12</v>
+      </c>
+      <c r="H222" s="3">
+        <f>schedule!D223</f>
+        <v>43427</v>
+      </c>
+      <c r="I222" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>9</v>
+      </c>
+      <c r="B223" t="str">
+        <f>schedule!A224</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C223" t="s">
+        <v>10</v>
+      </c>
+      <c r="D223">
+        <f>schedule!B224</f>
+        <v>68</v>
+      </c>
+      <c r="E223" t="s">
+        <v>11</v>
+      </c>
+      <c r="F223" s="2">
+        <f>schedule!C224</f>
+        <v>43413</v>
+      </c>
+      <c r="G223" t="s">
+        <v>12</v>
+      </c>
+      <c r="H223" s="3">
+        <f>schedule!D224</f>
+        <v>43441</v>
+      </c>
+      <c r="I223" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>9</v>
+      </c>
+      <c r="B224" t="str">
+        <f>schedule!A225</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C224" t="s">
+        <v>10</v>
+      </c>
+      <c r="D224">
+        <f>schedule!B225</f>
+        <v>68</v>
+      </c>
+      <c r="E224" t="s">
+        <v>11</v>
+      </c>
+      <c r="F224" s="2">
+        <f>schedule!C225</f>
+        <v>43427</v>
+      </c>
+      <c r="G224" t="s">
+        <v>12</v>
+      </c>
+      <c r="H224" s="3">
+        <f>schedule!D225</f>
+        <v>43455</v>
+      </c>
+      <c r="I224" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>9</v>
+      </c>
+      <c r="B225" t="str">
+        <f>schedule!A226</f>
+        <v>Trinys</v>
+      </c>
+      <c r="C225" t="s">
+        <v>10</v>
+      </c>
+      <c r="D225">
+        <f>schedule!B226</f>
+        <v>68</v>
+      </c>
+      <c r="E225" t="s">
+        <v>11</v>
+      </c>
+      <c r="F225" s="2">
+        <f>schedule!C226</f>
+        <v>43441</v>
+      </c>
+      <c r="G225" t="s">
+        <v>12</v>
+      </c>
+      <c r="H225" s="3">
+        <f>schedule!D226</f>
+        <v>43490</v>
+      </c>
+      <c r="I225" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>9</v>
+      </c>
+      <c r="B226" t="str">
+        <f>schedule!A227</f>
+        <v>Soles</v>
+      </c>
+      <c r="C226" t="s">
+        <v>10</v>
+      </c>
+      <c r="D226">
+        <f>schedule!B227</f>
+        <v>69</v>
+      </c>
+      <c r="E226" t="s">
+        <v>11</v>
+      </c>
+      <c r="F226" s="2">
+        <f>schedule!C227</f>
+        <v>43070</v>
+      </c>
+      <c r="G226" t="s">
+        <v>12</v>
+      </c>
+      <c r="H226" s="3">
+        <f>schedule!D227</f>
+        <v>43119</v>
+      </c>
+      <c r="I226" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>9</v>
+      </c>
+      <c r="B227" t="str">
+        <f>schedule!A228</f>
+        <v>Soles</v>
+      </c>
+      <c r="C227" t="s">
+        <v>10</v>
+      </c>
+      <c r="D227">
+        <f>schedule!B228</f>
+        <v>69</v>
+      </c>
+      <c r="E227" t="s">
+        <v>11</v>
+      </c>
+      <c r="F227" s="2">
+        <f>schedule!C228</f>
+        <v>43084</v>
+      </c>
+      <c r="G227" t="s">
+        <v>12</v>
+      </c>
+      <c r="H227" s="3">
+        <f>schedule!D228</f>
+        <v>43133</v>
+      </c>
+      <c r="I227" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>9</v>
+      </c>
+      <c r="B228" t="str">
+        <f>schedule!A229</f>
+        <v>Soles</v>
+      </c>
+      <c r="C228" t="s">
+        <v>10</v>
+      </c>
+      <c r="D228">
+        <f>schedule!B229</f>
+        <v>69</v>
+      </c>
+      <c r="E228" t="s">
+        <v>11</v>
+      </c>
+      <c r="F228" s="2">
+        <f>schedule!C229</f>
+        <v>43119</v>
+      </c>
+      <c r="G228" t="s">
+        <v>12</v>
+      </c>
+      <c r="H228" s="3">
+        <f>schedule!D229</f>
+        <v>43147</v>
+      </c>
+      <c r="I228" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>9</v>
+      </c>
+      <c r="B229" t="str">
+        <f>schedule!A230</f>
+        <v>Soles</v>
+      </c>
+      <c r="C229" t="s">
+        <v>10</v>
+      </c>
+      <c r="D229">
+        <f>schedule!B230</f>
+        <v>69</v>
+      </c>
+      <c r="E229" t="s">
+        <v>11</v>
+      </c>
+      <c r="F229" s="2">
+        <f>schedule!C230</f>
+        <v>43133</v>
+      </c>
+      <c r="G229" t="s">
+        <v>12</v>
+      </c>
+      <c r="H229" s="3">
+        <f>schedule!D230</f>
+        <v>43161</v>
+      </c>
+      <c r="I229" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>9</v>
+      </c>
+      <c r="B230" t="str">
+        <f>schedule!A231</f>
+        <v>Soles</v>
+      </c>
+      <c r="C230" t="s">
+        <v>10</v>
+      </c>
+      <c r="D230">
+        <f>schedule!B231</f>
+        <v>69</v>
+      </c>
+      <c r="E230" t="s">
+        <v>11</v>
+      </c>
+      <c r="F230" s="2">
+        <f>schedule!C231</f>
+        <v>43147</v>
+      </c>
+      <c r="G230" t="s">
+        <v>12</v>
+      </c>
+      <c r="H230" s="3">
+        <f>schedule!D231</f>
+        <v>43175</v>
+      </c>
+      <c r="I230" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>9</v>
+      </c>
+      <c r="B231" t="str">
+        <f>schedule!A232</f>
+        <v>Soles</v>
+      </c>
+      <c r="C231" t="s">
+        <v>10</v>
+      </c>
+      <c r="D231">
+        <f>schedule!B232</f>
+        <v>69</v>
+      </c>
+      <c r="E231" t="s">
+        <v>11</v>
+      </c>
+      <c r="F231" s="2">
+        <f>schedule!C232</f>
+        <v>43161</v>
+      </c>
+      <c r="G231" t="s">
+        <v>12</v>
+      </c>
+      <c r="H231" s="3">
+        <f>schedule!D232</f>
+        <v>43189</v>
+      </c>
+      <c r="I231" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>9</v>
+      </c>
+      <c r="B232" t="str">
+        <f>schedule!A233</f>
+        <v>Soles</v>
+      </c>
+      <c r="C232" t="s">
+        <v>10</v>
+      </c>
+      <c r="D232">
+        <f>schedule!B233</f>
+        <v>69</v>
+      </c>
+      <c r="E232" t="s">
+        <v>11</v>
+      </c>
+      <c r="F232" s="2">
+        <f>schedule!C233</f>
+        <v>43175</v>
+      </c>
+      <c r="G232" t="s">
+        <v>12</v>
+      </c>
+      <c r="H232" s="3">
+        <f>schedule!D233</f>
+        <v>43203</v>
+      </c>
+      <c r="I232" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>9</v>
+      </c>
+      <c r="B233" t="str">
+        <f>schedule!A234</f>
+        <v>Soles</v>
+      </c>
+      <c r="C233" t="s">
+        <v>10</v>
+      </c>
+      <c r="D233">
+        <f>schedule!B234</f>
+        <v>69</v>
+      </c>
+      <c r="E233" t="s">
+        <v>11</v>
+      </c>
+      <c r="F233" s="2">
+        <f>schedule!C234</f>
+        <v>43189</v>
+      </c>
+      <c r="G233" t="s">
+        <v>12</v>
+      </c>
+      <c r="H233" s="3">
+        <f>schedule!D234</f>
+        <v>43217</v>
+      </c>
+      <c r="I233" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>9</v>
+      </c>
+      <c r="B234" t="str">
+        <f>schedule!A235</f>
+        <v>Soles</v>
+      </c>
+      <c r="C234" t="s">
+        <v>10</v>
+      </c>
+      <c r="D234">
+        <f>schedule!B235</f>
+        <v>69</v>
+      </c>
+      <c r="E234" t="s">
+        <v>11</v>
+      </c>
+      <c r="F234" s="2">
+        <f>schedule!C235</f>
+        <v>43203</v>
+      </c>
+      <c r="G234" t="s">
+        <v>12</v>
+      </c>
+      <c r="H234" s="3">
+        <f>schedule!D235</f>
+        <v>43231</v>
+      </c>
+      <c r="I234" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>9</v>
+      </c>
+      <c r="B235" t="str">
+        <f>schedule!A236</f>
+        <v>Soles</v>
+      </c>
+      <c r="C235" t="s">
+        <v>10</v>
+      </c>
+      <c r="D235">
+        <f>schedule!B236</f>
+        <v>69</v>
+      </c>
+      <c r="E235" t="s">
+        <v>11</v>
+      </c>
+      <c r="F235" s="2">
+        <f>schedule!C236</f>
+        <v>43217</v>
+      </c>
+      <c r="G235" t="s">
+        <v>12</v>
+      </c>
+      <c r="H235" s="3">
+        <f>schedule!D236</f>
+        <v>43245</v>
+      </c>
+      <c r="I235" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>9</v>
+      </c>
+      <c r="B236" t="str">
+        <f>schedule!A237</f>
+        <v>Soles</v>
+      </c>
+      <c r="C236" t="s">
+        <v>10</v>
+      </c>
+      <c r="D236">
+        <f>schedule!B237</f>
+        <v>69</v>
+      </c>
+      <c r="E236" t="s">
+        <v>11</v>
+      </c>
+      <c r="F236" s="2">
+        <f>schedule!C237</f>
+        <v>43231</v>
+      </c>
+      <c r="G236" t="s">
+        <v>12</v>
+      </c>
+      <c r="H236" s="3">
+        <f>schedule!D237</f>
+        <v>43259</v>
+      </c>
+      <c r="I236" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>9</v>
+      </c>
+      <c r="B237" t="str">
+        <f>schedule!A238</f>
+        <v>Soles</v>
+      </c>
+      <c r="C237" t="s">
+        <v>10</v>
+      </c>
+      <c r="D237">
+        <f>schedule!B238</f>
+        <v>69</v>
+      </c>
+      <c r="E237" t="s">
+        <v>11</v>
+      </c>
+      <c r="F237" s="2">
+        <f>schedule!C238</f>
+        <v>43245</v>
+      </c>
+      <c r="G237" t="s">
+        <v>12</v>
+      </c>
+      <c r="H237" s="3">
+        <f>schedule!D238</f>
+        <v>43273</v>
+      </c>
+      <c r="I237" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>9</v>
+      </c>
+      <c r="B238" t="str">
+        <f>schedule!A239</f>
+        <v>Soles</v>
+      </c>
+      <c r="C238" t="s">
+        <v>10</v>
+      </c>
+      <c r="D238">
+        <f>schedule!B239</f>
+        <v>69</v>
+      </c>
+      <c r="E238" t="s">
+        <v>11</v>
+      </c>
+      <c r="F238" s="2">
+        <f>schedule!C239</f>
+        <v>43259</v>
+      </c>
+      <c r="G238" t="s">
+        <v>12</v>
+      </c>
+      <c r="H238" s="3">
+        <f>schedule!D239</f>
+        <v>43271</v>
+      </c>
+      <c r="I238" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>9</v>
+      </c>
+      <c r="B239" t="str">
+        <f>schedule!A240</f>
+        <v>Soles</v>
+      </c>
+      <c r="C239" t="s">
+        <v>10</v>
+      </c>
+      <c r="D239">
+        <f>schedule!B240</f>
+        <v>69</v>
+      </c>
+      <c r="E239" t="s">
+        <v>11</v>
+      </c>
+      <c r="F239" s="2">
+        <f>schedule!C240</f>
+        <v>43273</v>
+      </c>
+      <c r="G239" t="s">
+        <v>12</v>
+      </c>
+      <c r="H239" s="3">
+        <f>schedule!D240</f>
+        <v>43315</v>
+      </c>
+      <c r="I239" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>9</v>
+      </c>
+      <c r="B240" t="str">
+        <f>schedule!A241</f>
+        <v>Soles</v>
+      </c>
+      <c r="C240" t="s">
+        <v>10</v>
+      </c>
+      <c r="D240">
+        <f>schedule!B241</f>
+        <v>69</v>
+      </c>
+      <c r="E240" t="s">
+        <v>11</v>
+      </c>
+      <c r="F240" s="2">
+        <f>schedule!C241</f>
+        <v>43271</v>
+      </c>
+      <c r="G240" t="s">
+        <v>12</v>
+      </c>
+      <c r="H240" s="3">
+        <f>schedule!D241</f>
+        <v>43329</v>
+      </c>
+      <c r="I240" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>9</v>
+      </c>
+      <c r="B241" t="str">
+        <f>schedule!A242</f>
+        <v>Soles</v>
+      </c>
+      <c r="C241" t="s">
+        <v>10</v>
+      </c>
+      <c r="D241">
+        <f>schedule!B242</f>
+        <v>69</v>
+      </c>
+      <c r="E241" t="s">
+        <v>11</v>
+      </c>
+      <c r="F241" s="2">
+        <f>schedule!C242</f>
+        <v>43315</v>
+      </c>
+      <c r="G241" t="s">
+        <v>12</v>
+      </c>
+      <c r="H241" s="3">
+        <f>schedule!D242</f>
+        <v>43343</v>
+      </c>
+      <c r="I241" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>9</v>
+      </c>
+      <c r="B242" t="str">
+        <f>schedule!A243</f>
+        <v>Soles</v>
+      </c>
+      <c r="C242" t="s">
+        <v>10</v>
+      </c>
+      <c r="D242">
+        <f>schedule!B243</f>
+        <v>69</v>
+      </c>
+      <c r="E242" t="s">
+        <v>11</v>
+      </c>
+      <c r="F242" s="2">
+        <f>schedule!C243</f>
+        <v>43329</v>
+      </c>
+      <c r="G242" t="s">
+        <v>12</v>
+      </c>
+      <c r="H242" s="3">
+        <f>schedule!D243</f>
+        <v>43357</v>
+      </c>
+      <c r="I242" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>9</v>
+      </c>
+      <c r="B243" t="str">
+        <f>schedule!A244</f>
+        <v>Soles</v>
+      </c>
+      <c r="C243" t="s">
+        <v>10</v>
+      </c>
+      <c r="D243">
+        <f>schedule!B244</f>
+        <v>69</v>
+      </c>
+      <c r="E243" t="s">
+        <v>11</v>
+      </c>
+      <c r="F243" s="2">
+        <f>schedule!C244</f>
+        <v>43343</v>
+      </c>
+      <c r="G243" t="s">
+        <v>12</v>
+      </c>
+      <c r="H243" s="3">
+        <f>schedule!D244</f>
+        <v>43371</v>
+      </c>
+      <c r="I243" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>9</v>
+      </c>
+      <c r="B244" t="str">
+        <f>schedule!A245</f>
+        <v>Soles</v>
+      </c>
+      <c r="C244" t="s">
+        <v>10</v>
+      </c>
+      <c r="D244">
+        <f>schedule!B245</f>
+        <v>69</v>
+      </c>
+      <c r="E244" t="s">
+        <v>11</v>
+      </c>
+      <c r="F244" s="2">
+        <f>schedule!C245</f>
+        <v>43357</v>
+      </c>
+      <c r="G244" t="s">
+        <v>12</v>
+      </c>
+      <c r="H244" s="3">
+        <f>schedule!D245</f>
+        <v>43385</v>
+      </c>
+      <c r="I244" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>9</v>
+      </c>
+      <c r="B245" t="str">
+        <f>schedule!A246</f>
+        <v>Soles</v>
+      </c>
+      <c r="C245" t="s">
+        <v>10</v>
+      </c>
+      <c r="D245">
+        <f>schedule!B246</f>
+        <v>69</v>
+      </c>
+      <c r="E245" t="s">
+        <v>11</v>
+      </c>
+      <c r="F245" s="2">
+        <f>schedule!C246</f>
+        <v>43371</v>
+      </c>
+      <c r="G245" t="s">
+        <v>12</v>
+      </c>
+      <c r="H245" s="3">
+        <f>schedule!D246</f>
+        <v>43399</v>
+      </c>
+      <c r="I245" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>9</v>
+      </c>
+      <c r="B246" t="str">
+        <f>schedule!A247</f>
+        <v>Soles</v>
+      </c>
+      <c r="C246" t="s">
+        <v>10</v>
+      </c>
+      <c r="D246">
+        <f>schedule!B247</f>
+        <v>69</v>
+      </c>
+      <c r="E246" t="s">
+        <v>11</v>
+      </c>
+      <c r="F246" s="2">
+        <f>schedule!C247</f>
+        <v>43385</v>
+      </c>
+      <c r="G246" t="s">
+        <v>12</v>
+      </c>
+      <c r="H246" s="3">
+        <f>schedule!D247</f>
+        <v>43413</v>
+      </c>
+      <c r="I246" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>9</v>
+      </c>
+      <c r="B247" t="str">
+        <f>schedule!A248</f>
+        <v>Soles</v>
+      </c>
+      <c r="C247" t="s">
+        <v>10</v>
+      </c>
+      <c r="D247">
+        <f>schedule!B248</f>
+        <v>69</v>
+      </c>
+      <c r="E247" t="s">
+        <v>11</v>
+      </c>
+      <c r="F247" s="2">
+        <f>schedule!C248</f>
+        <v>43399</v>
+      </c>
+      <c r="G247" t="s">
+        <v>12</v>
+      </c>
+      <c r="H247" s="3">
+        <f>schedule!D248</f>
+        <v>43427</v>
+      </c>
+      <c r="I247" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>9</v>
+      </c>
+      <c r="B248" t="str">
+        <f>schedule!A249</f>
+        <v>Soles</v>
+      </c>
+      <c r="C248" t="s">
+        <v>10</v>
+      </c>
+      <c r="D248">
+        <f>schedule!B249</f>
+        <v>69</v>
+      </c>
+      <c r="E248" t="s">
+        <v>11</v>
+      </c>
+      <c r="F248" s="2">
+        <f>schedule!C249</f>
+        <v>43413</v>
+      </c>
+      <c r="G248" t="s">
+        <v>12</v>
+      </c>
+      <c r="H248" s="3">
+        <f>schedule!D249</f>
+        <v>43441</v>
+      </c>
+      <c r="I248" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>9</v>
+      </c>
+      <c r="B249" t="str">
+        <f>schedule!A250</f>
+        <v>Soles</v>
+      </c>
+      <c r="C249" t="s">
+        <v>10</v>
+      </c>
+      <c r="D249">
+        <f>schedule!B250</f>
+        <v>69</v>
+      </c>
+      <c r="E249" t="s">
+        <v>11</v>
+      </c>
+      <c r="F249" s="2">
+        <f>schedule!C250</f>
+        <v>43427</v>
+      </c>
+      <c r="G249" t="s">
+        <v>12</v>
+      </c>
+      <c r="H249" s="3">
+        <f>schedule!D250</f>
+        <v>43455</v>
+      </c>
+      <c r="I249" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>9</v>
+      </c>
+      <c r="B250" t="str">
+        <f>schedule!A251</f>
+        <v>Soles</v>
+      </c>
+      <c r="C250" t="s">
+        <v>10</v>
+      </c>
+      <c r="D250">
+        <f>schedule!B251</f>
+        <v>69</v>
+      </c>
+      <c r="E250" t="s">
+        <v>11</v>
+      </c>
+      <c r="F250" s="2">
+        <f>schedule!C251</f>
+        <v>43441</v>
+      </c>
+      <c r="G250" t="s">
+        <v>12</v>
+      </c>
+      <c r="H250" s="3">
+        <f>schedule!D251</f>
+        <v>43490</v>
+      </c>
+      <c r="I250" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -10301,10 +12581,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A200"/>
+  <dimension ref="A1:A250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="A251" sqref="A251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11510,6 +13790,306 @@
       <c r="A200" t="str">
         <f>sql_raw!A200&amp;sql_raw!B200&amp;sql_raw!C200&amp;sql_raw!D200&amp;sql_raw!E200&amp;TEXT(sql_raw!F200,"yyyy-mm-dd")&amp;sql_raw!G200&amp;TEXT(sql_raw!H200,"yyyy-mm-dd")&amp;sql_raw!I200</f>
         <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Private Label',20125,'2018-12-07','2019-01-25');</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="str">
+        <f>sql_raw!A201&amp;sql_raw!B201&amp;sql_raw!C201&amp;sql_raw!D201&amp;sql_raw!E201&amp;TEXT(sql_raw!F201,"yyyy-mm-dd")&amp;sql_raw!G201&amp;TEXT(sql_raw!H201,"yyyy-mm-dd")&amp;sql_raw!I201</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2017-12-01','2018-01-19');</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="str">
+        <f>sql_raw!A202&amp;sql_raw!B202&amp;sql_raw!C202&amp;sql_raw!D202&amp;sql_raw!E202&amp;TEXT(sql_raw!F202,"yyyy-mm-dd")&amp;sql_raw!G202&amp;TEXT(sql_raw!H202,"yyyy-mm-dd")&amp;sql_raw!I202</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2017-12-15','2018-02-02');</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="str">
+        <f>sql_raw!A203&amp;sql_raw!B203&amp;sql_raw!C203&amp;sql_raw!D203&amp;sql_raw!E203&amp;TEXT(sql_raw!F203,"yyyy-mm-dd")&amp;sql_raw!G203&amp;TEXT(sql_raw!H203,"yyyy-mm-dd")&amp;sql_raw!I203</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-01-19','2018-02-16');</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="str">
+        <f>sql_raw!A204&amp;sql_raw!B204&amp;sql_raw!C204&amp;sql_raw!D204&amp;sql_raw!E204&amp;TEXT(sql_raw!F204,"yyyy-mm-dd")&amp;sql_raw!G204&amp;TEXT(sql_raw!H204,"yyyy-mm-dd")&amp;sql_raw!I204</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-02-02','2018-03-02');</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="str">
+        <f>sql_raw!A205&amp;sql_raw!B205&amp;sql_raw!C205&amp;sql_raw!D205&amp;sql_raw!E205&amp;TEXT(sql_raw!F205,"yyyy-mm-dd")&amp;sql_raw!G205&amp;TEXT(sql_raw!H205,"yyyy-mm-dd")&amp;sql_raw!I205</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-02-16','2018-03-16');</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="str">
+        <f>sql_raw!A206&amp;sql_raw!B206&amp;sql_raw!C206&amp;sql_raw!D206&amp;sql_raw!E206&amp;TEXT(sql_raw!F206,"yyyy-mm-dd")&amp;sql_raw!G206&amp;TEXT(sql_raw!H206,"yyyy-mm-dd")&amp;sql_raw!I206</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-03-02','2018-03-30');</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="str">
+        <f>sql_raw!A207&amp;sql_raw!B207&amp;sql_raw!C207&amp;sql_raw!D207&amp;sql_raw!E207&amp;TEXT(sql_raw!F207,"yyyy-mm-dd")&amp;sql_raw!G207&amp;TEXT(sql_raw!H207,"yyyy-mm-dd")&amp;sql_raw!I207</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-03-16','2018-04-13');</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="str">
+        <f>sql_raw!A208&amp;sql_raw!B208&amp;sql_raw!C208&amp;sql_raw!D208&amp;sql_raw!E208&amp;TEXT(sql_raw!F208,"yyyy-mm-dd")&amp;sql_raw!G208&amp;TEXT(sql_raw!H208,"yyyy-mm-dd")&amp;sql_raw!I208</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-03-30','2018-04-27');</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="str">
+        <f>sql_raw!A209&amp;sql_raw!B209&amp;sql_raw!C209&amp;sql_raw!D209&amp;sql_raw!E209&amp;TEXT(sql_raw!F209,"yyyy-mm-dd")&amp;sql_raw!G209&amp;TEXT(sql_raw!H209,"yyyy-mm-dd")&amp;sql_raw!I209</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-04-13','2018-05-11');</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="str">
+        <f>sql_raw!A210&amp;sql_raw!B210&amp;sql_raw!C210&amp;sql_raw!D210&amp;sql_raw!E210&amp;TEXT(sql_raw!F210,"yyyy-mm-dd")&amp;sql_raw!G210&amp;TEXT(sql_raw!H210,"yyyy-mm-dd")&amp;sql_raw!I210</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-04-27','2018-05-25');</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="str">
+        <f>sql_raw!A211&amp;sql_raw!B211&amp;sql_raw!C211&amp;sql_raw!D211&amp;sql_raw!E211&amp;TEXT(sql_raw!F211,"yyyy-mm-dd")&amp;sql_raw!G211&amp;TEXT(sql_raw!H211,"yyyy-mm-dd")&amp;sql_raw!I211</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-05-11','2018-06-08');</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="str">
+        <f>sql_raw!A212&amp;sql_raw!B212&amp;sql_raw!C212&amp;sql_raw!D212&amp;sql_raw!E212&amp;TEXT(sql_raw!F212,"yyyy-mm-dd")&amp;sql_raw!G212&amp;TEXT(sql_raw!H212,"yyyy-mm-dd")&amp;sql_raw!I212</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-05-25','2018-06-22');</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="str">
+        <f>sql_raw!A213&amp;sql_raw!B213&amp;sql_raw!C213&amp;sql_raw!D213&amp;sql_raw!E213&amp;TEXT(sql_raw!F213,"yyyy-mm-dd")&amp;sql_raw!G213&amp;TEXT(sql_raw!H213,"yyyy-mm-dd")&amp;sql_raw!I213</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-06-08','2018-06-20');</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="str">
+        <f>sql_raw!A214&amp;sql_raw!B214&amp;sql_raw!C214&amp;sql_raw!D214&amp;sql_raw!E214&amp;TEXT(sql_raw!F214,"yyyy-mm-dd")&amp;sql_raw!G214&amp;TEXT(sql_raw!H214,"yyyy-mm-dd")&amp;sql_raw!I214</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-06-22','2018-08-03');</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="str">
+        <f>sql_raw!A215&amp;sql_raw!B215&amp;sql_raw!C215&amp;sql_raw!D215&amp;sql_raw!E215&amp;TEXT(sql_raw!F215,"yyyy-mm-dd")&amp;sql_raw!G215&amp;TEXT(sql_raw!H215,"yyyy-mm-dd")&amp;sql_raw!I215</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-06-20','2018-08-17');</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="str">
+        <f>sql_raw!A216&amp;sql_raw!B216&amp;sql_raw!C216&amp;sql_raw!D216&amp;sql_raw!E216&amp;TEXT(sql_raw!F216,"yyyy-mm-dd")&amp;sql_raw!G216&amp;TEXT(sql_raw!H216,"yyyy-mm-dd")&amp;sql_raw!I216</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-08-03','2018-08-31');</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="str">
+        <f>sql_raw!A217&amp;sql_raw!B217&amp;sql_raw!C217&amp;sql_raw!D217&amp;sql_raw!E217&amp;TEXT(sql_raw!F217,"yyyy-mm-dd")&amp;sql_raw!G217&amp;TEXT(sql_raw!H217,"yyyy-mm-dd")&amp;sql_raw!I217</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-08-17','2018-09-14');</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="str">
+        <f>sql_raw!A218&amp;sql_raw!B218&amp;sql_raw!C218&amp;sql_raw!D218&amp;sql_raw!E218&amp;TEXT(sql_raw!F218,"yyyy-mm-dd")&amp;sql_raw!G218&amp;TEXT(sql_raw!H218,"yyyy-mm-dd")&amp;sql_raw!I218</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-08-31','2018-09-28');</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="str">
+        <f>sql_raw!A219&amp;sql_raw!B219&amp;sql_raw!C219&amp;sql_raw!D219&amp;sql_raw!E219&amp;TEXT(sql_raw!F219,"yyyy-mm-dd")&amp;sql_raw!G219&amp;TEXT(sql_raw!H219,"yyyy-mm-dd")&amp;sql_raw!I219</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-09-14','2018-10-12');</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="str">
+        <f>sql_raw!A220&amp;sql_raw!B220&amp;sql_raw!C220&amp;sql_raw!D220&amp;sql_raw!E220&amp;TEXT(sql_raw!F220,"yyyy-mm-dd")&amp;sql_raw!G220&amp;TEXT(sql_raw!H220,"yyyy-mm-dd")&amp;sql_raw!I220</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-09-28','2018-10-26');</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="str">
+        <f>sql_raw!A221&amp;sql_raw!B221&amp;sql_raw!C221&amp;sql_raw!D221&amp;sql_raw!E221&amp;TEXT(sql_raw!F221,"yyyy-mm-dd")&amp;sql_raw!G221&amp;TEXT(sql_raw!H221,"yyyy-mm-dd")&amp;sql_raw!I221</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-10-12','2018-11-09');</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="str">
+        <f>sql_raw!A222&amp;sql_raw!B222&amp;sql_raw!C222&amp;sql_raw!D222&amp;sql_raw!E222&amp;TEXT(sql_raw!F222,"yyyy-mm-dd")&amp;sql_raw!G222&amp;TEXT(sql_raw!H222,"yyyy-mm-dd")&amp;sql_raw!I222</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-10-26','2018-11-23');</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="str">
+        <f>sql_raw!A223&amp;sql_raw!B223&amp;sql_raw!C223&amp;sql_raw!D223&amp;sql_raw!E223&amp;TEXT(sql_raw!F223,"yyyy-mm-dd")&amp;sql_raw!G223&amp;TEXT(sql_raw!H223,"yyyy-mm-dd")&amp;sql_raw!I223</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-11-09','2018-12-07');</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="str">
+        <f>sql_raw!A224&amp;sql_raw!B224&amp;sql_raw!C224&amp;sql_raw!D224&amp;sql_raw!E224&amp;TEXT(sql_raw!F224,"yyyy-mm-dd")&amp;sql_raw!G224&amp;TEXT(sql_raw!H224,"yyyy-mm-dd")&amp;sql_raw!I224</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-11-23','2018-12-21');</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="str">
+        <f>sql_raw!A225&amp;sql_raw!B225&amp;sql_raw!C225&amp;sql_raw!D225&amp;sql_raw!E225&amp;TEXT(sql_raw!F225,"yyyy-mm-dd")&amp;sql_raw!G225&amp;TEXT(sql_raw!H225,"yyyy-mm-dd")&amp;sql_raw!I225</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Trinys',68,'2018-12-07','2019-01-25');</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="str">
+        <f>sql_raw!A226&amp;sql_raw!B226&amp;sql_raw!C226&amp;sql_raw!D226&amp;sql_raw!E226&amp;TEXT(sql_raw!F226,"yyyy-mm-dd")&amp;sql_raw!G226&amp;TEXT(sql_raw!H226,"yyyy-mm-dd")&amp;sql_raw!I226</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2017-12-01','2018-01-19');</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="str">
+        <f>sql_raw!A227&amp;sql_raw!B227&amp;sql_raw!C227&amp;sql_raw!D227&amp;sql_raw!E227&amp;TEXT(sql_raw!F227,"yyyy-mm-dd")&amp;sql_raw!G227&amp;TEXT(sql_raw!H227,"yyyy-mm-dd")&amp;sql_raw!I227</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2017-12-15','2018-02-02');</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="str">
+        <f>sql_raw!A228&amp;sql_raw!B228&amp;sql_raw!C228&amp;sql_raw!D228&amp;sql_raw!E228&amp;TEXT(sql_raw!F228,"yyyy-mm-dd")&amp;sql_raw!G228&amp;TEXT(sql_raw!H228,"yyyy-mm-dd")&amp;sql_raw!I228</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-01-19','2018-02-16');</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="str">
+        <f>sql_raw!A229&amp;sql_raw!B229&amp;sql_raw!C229&amp;sql_raw!D229&amp;sql_raw!E229&amp;TEXT(sql_raw!F229,"yyyy-mm-dd")&amp;sql_raw!G229&amp;TEXT(sql_raw!H229,"yyyy-mm-dd")&amp;sql_raw!I229</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-02-02','2018-03-02');</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="str">
+        <f>sql_raw!A230&amp;sql_raw!B230&amp;sql_raw!C230&amp;sql_raw!D230&amp;sql_raw!E230&amp;TEXT(sql_raw!F230,"yyyy-mm-dd")&amp;sql_raw!G230&amp;TEXT(sql_raw!H230,"yyyy-mm-dd")&amp;sql_raw!I230</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-02-16','2018-03-16');</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="str">
+        <f>sql_raw!A231&amp;sql_raw!B231&amp;sql_raw!C231&amp;sql_raw!D231&amp;sql_raw!E231&amp;TEXT(sql_raw!F231,"yyyy-mm-dd")&amp;sql_raw!G231&amp;TEXT(sql_raw!H231,"yyyy-mm-dd")&amp;sql_raw!I231</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-03-02','2018-03-30');</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="str">
+        <f>sql_raw!A232&amp;sql_raw!B232&amp;sql_raw!C232&amp;sql_raw!D232&amp;sql_raw!E232&amp;TEXT(sql_raw!F232,"yyyy-mm-dd")&amp;sql_raw!G232&amp;TEXT(sql_raw!H232,"yyyy-mm-dd")&amp;sql_raw!I232</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-03-16','2018-04-13');</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="str">
+        <f>sql_raw!A233&amp;sql_raw!B233&amp;sql_raw!C233&amp;sql_raw!D233&amp;sql_raw!E233&amp;TEXT(sql_raw!F233,"yyyy-mm-dd")&amp;sql_raw!G233&amp;TEXT(sql_raw!H233,"yyyy-mm-dd")&amp;sql_raw!I233</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-03-30','2018-04-27');</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="str">
+        <f>sql_raw!A234&amp;sql_raw!B234&amp;sql_raw!C234&amp;sql_raw!D234&amp;sql_raw!E234&amp;TEXT(sql_raw!F234,"yyyy-mm-dd")&amp;sql_raw!G234&amp;TEXT(sql_raw!H234,"yyyy-mm-dd")&amp;sql_raw!I234</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-04-13','2018-05-11');</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="str">
+        <f>sql_raw!A235&amp;sql_raw!B235&amp;sql_raw!C235&amp;sql_raw!D235&amp;sql_raw!E235&amp;TEXT(sql_raw!F235,"yyyy-mm-dd")&amp;sql_raw!G235&amp;TEXT(sql_raw!H235,"yyyy-mm-dd")&amp;sql_raw!I235</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-04-27','2018-05-25');</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="str">
+        <f>sql_raw!A236&amp;sql_raw!B236&amp;sql_raw!C236&amp;sql_raw!D236&amp;sql_raw!E236&amp;TEXT(sql_raw!F236,"yyyy-mm-dd")&amp;sql_raw!G236&amp;TEXT(sql_raw!H236,"yyyy-mm-dd")&amp;sql_raw!I236</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-05-11','2018-06-08');</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" t="str">
+        <f>sql_raw!A237&amp;sql_raw!B237&amp;sql_raw!C237&amp;sql_raw!D237&amp;sql_raw!E237&amp;TEXT(sql_raw!F237,"yyyy-mm-dd")&amp;sql_raw!G237&amp;TEXT(sql_raw!H237,"yyyy-mm-dd")&amp;sql_raw!I237</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-05-25','2018-06-22');</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" t="str">
+        <f>sql_raw!A238&amp;sql_raw!B238&amp;sql_raw!C238&amp;sql_raw!D238&amp;sql_raw!E238&amp;TEXT(sql_raw!F238,"yyyy-mm-dd")&amp;sql_raw!G238&amp;TEXT(sql_raw!H238,"yyyy-mm-dd")&amp;sql_raw!I238</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-06-08','2018-06-20');</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" t="str">
+        <f>sql_raw!A239&amp;sql_raw!B239&amp;sql_raw!C239&amp;sql_raw!D239&amp;sql_raw!E239&amp;TEXT(sql_raw!F239,"yyyy-mm-dd")&amp;sql_raw!G239&amp;TEXT(sql_raw!H239,"yyyy-mm-dd")&amp;sql_raw!I239</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-06-22','2018-08-03');</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" t="str">
+        <f>sql_raw!A240&amp;sql_raw!B240&amp;sql_raw!C240&amp;sql_raw!D240&amp;sql_raw!E240&amp;TEXT(sql_raw!F240,"yyyy-mm-dd")&amp;sql_raw!G240&amp;TEXT(sql_raw!H240,"yyyy-mm-dd")&amp;sql_raw!I240</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-06-20','2018-08-17');</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" t="str">
+        <f>sql_raw!A241&amp;sql_raw!B241&amp;sql_raw!C241&amp;sql_raw!D241&amp;sql_raw!E241&amp;TEXT(sql_raw!F241,"yyyy-mm-dd")&amp;sql_raw!G241&amp;TEXT(sql_raw!H241,"yyyy-mm-dd")&amp;sql_raw!I241</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-08-03','2018-08-31');</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" t="str">
+        <f>sql_raw!A242&amp;sql_raw!B242&amp;sql_raw!C242&amp;sql_raw!D242&amp;sql_raw!E242&amp;TEXT(sql_raw!F242,"yyyy-mm-dd")&amp;sql_raw!G242&amp;TEXT(sql_raw!H242,"yyyy-mm-dd")&amp;sql_raw!I242</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-08-17','2018-09-14');</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" t="str">
+        <f>sql_raw!A243&amp;sql_raw!B243&amp;sql_raw!C243&amp;sql_raw!D243&amp;sql_raw!E243&amp;TEXT(sql_raw!F243,"yyyy-mm-dd")&amp;sql_raw!G243&amp;TEXT(sql_raw!H243,"yyyy-mm-dd")&amp;sql_raw!I243</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-08-31','2018-09-28');</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" t="str">
+        <f>sql_raw!A244&amp;sql_raw!B244&amp;sql_raw!C244&amp;sql_raw!D244&amp;sql_raw!E244&amp;TEXT(sql_raw!F244,"yyyy-mm-dd")&amp;sql_raw!G244&amp;TEXT(sql_raw!H244,"yyyy-mm-dd")&amp;sql_raw!I244</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-09-14','2018-10-12');</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" t="str">
+        <f>sql_raw!A245&amp;sql_raw!B245&amp;sql_raw!C245&amp;sql_raw!D245&amp;sql_raw!E245&amp;TEXT(sql_raw!F245,"yyyy-mm-dd")&amp;sql_raw!G245&amp;TEXT(sql_raw!H245,"yyyy-mm-dd")&amp;sql_raw!I245</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-09-28','2018-10-26');</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" t="str">
+        <f>sql_raw!A246&amp;sql_raw!B246&amp;sql_raw!C246&amp;sql_raw!D246&amp;sql_raw!E246&amp;TEXT(sql_raw!F246,"yyyy-mm-dd")&amp;sql_raw!G246&amp;TEXT(sql_raw!H246,"yyyy-mm-dd")&amp;sql_raw!I246</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-10-12','2018-11-09');</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" t="str">
+        <f>sql_raw!A247&amp;sql_raw!B247&amp;sql_raw!C247&amp;sql_raw!D247&amp;sql_raw!E247&amp;TEXT(sql_raw!F247,"yyyy-mm-dd")&amp;sql_raw!G247&amp;TEXT(sql_raw!H247,"yyyy-mm-dd")&amp;sql_raw!I247</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-10-26','2018-11-23');</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" t="str">
+        <f>sql_raw!A248&amp;sql_raw!B248&amp;sql_raw!C248&amp;sql_raw!D248&amp;sql_raw!E248&amp;TEXT(sql_raw!F248,"yyyy-mm-dd")&amp;sql_raw!G248&amp;TEXT(sql_raw!H248,"yyyy-mm-dd")&amp;sql_raw!I248</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-11-09','2018-12-07');</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" t="str">
+        <f>sql_raw!A249&amp;sql_raw!B249&amp;sql_raw!C249&amp;sql_raw!D249&amp;sql_raw!E249&amp;TEXT(sql_raw!F249,"yyyy-mm-dd")&amp;sql_raw!G249&amp;TEXT(sql_raw!H249,"yyyy-mm-dd")&amp;sql_raw!I249</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-11-23','2018-12-21');</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" t="str">
+        <f>sql_raw!A250&amp;sql_raw!B250&amp;sql_raw!C250&amp;sql_raw!D250&amp;sql_raw!E250&amp;TEXT(sql_raw!F250,"yyyy-mm-dd")&amp;sql_raw!G250&amp;TEXT(sql_raw!H250,"yyyy-mm-dd")&amp;sql_raw!I250</f>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles',69,'2018-12-07','2019-01-25');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating spreadshee and sql  schedule files
</commit_message>
<xml_diff>
--- a/PurchaseOrder_Scheduler/schedule_insert_spreadsheet.xlsx
+++ b/PurchaseOrder_Scheduler/schedule_insert_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipe\Documents\purchase_planner\PurchaseOrder_Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{841F9F8A-390C-44F5-A4C3-A39FC00C6218}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6D46C8-79D4-4F1B-A502-FAD597294F86}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102:B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2104,7 +2104,7 @@
         <v>28</v>
       </c>
       <c r="B103">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C103" s="1">
         <v>43084</v>
@@ -2118,7 +2118,7 @@
         <v>28</v>
       </c>
       <c r="B104">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C104" s="1">
         <v>43119</v>
@@ -2132,7 +2132,7 @@
         <v>28</v>
       </c>
       <c r="B105">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C105" s="1">
         <v>43133</v>
@@ -2146,7 +2146,7 @@
         <v>28</v>
       </c>
       <c r="B106">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C106" s="1">
         <v>43147</v>
@@ -2161,7 +2161,7 @@
         <v>28</v>
       </c>
       <c r="B107">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C107" s="1">
         <v>43161</v>
@@ -2176,7 +2176,7 @@
         <v>28</v>
       </c>
       <c r="B108">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C108" s="1">
         <v>43175</v>
@@ -2191,7 +2191,7 @@
         <v>28</v>
       </c>
       <c r="B109">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C109" s="1">
         <v>43189</v>
@@ -2206,7 +2206,7 @@
         <v>28</v>
       </c>
       <c r="B110">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C110" s="1">
         <v>43203</v>
@@ -2221,7 +2221,7 @@
         <v>28</v>
       </c>
       <c r="B111">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C111" s="1">
         <v>43217</v>
@@ -2236,7 +2236,7 @@
         <v>28</v>
       </c>
       <c r="B112">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C112" s="1">
         <v>43231</v>
@@ -2251,7 +2251,7 @@
         <v>28</v>
       </c>
       <c r="B113">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C113" s="1">
         <v>43245</v>
@@ -2266,7 +2266,7 @@
         <v>28</v>
       </c>
       <c r="B114">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C114" s="1">
         <v>43259</v>
@@ -2281,7 +2281,7 @@
         <v>28</v>
       </c>
       <c r="B115">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C115" s="1">
         <v>43273</v>
@@ -2296,7 +2296,7 @@
         <v>28</v>
       </c>
       <c r="B116">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C116" s="1">
         <v>43271</v>
@@ -2311,7 +2311,7 @@
         <v>28</v>
       </c>
       <c r="B117">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C117" s="1">
         <v>43315</v>
@@ -2326,7 +2326,7 @@
         <v>28</v>
       </c>
       <c r="B118">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C118" s="1">
         <v>43329</v>
@@ -2341,7 +2341,7 @@
         <v>28</v>
       </c>
       <c r="B119">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C119" s="1">
         <v>43343</v>
@@ -2356,7 +2356,7 @@
         <v>28</v>
       </c>
       <c r="B120">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C120" s="1">
         <v>43357</v>
@@ -2371,7 +2371,7 @@
         <v>28</v>
       </c>
       <c r="B121">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C121" s="1">
         <v>43371</v>
@@ -2386,7 +2386,7 @@
         <v>28</v>
       </c>
       <c r="B122">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C122" s="1">
         <v>43385</v>
@@ -2401,7 +2401,7 @@
         <v>28</v>
       </c>
       <c r="B123">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C123" s="1">
         <v>43399</v>
@@ -2416,7 +2416,7 @@
         <v>28</v>
       </c>
       <c r="B124">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C124" s="1">
         <v>43413</v>
@@ -2431,7 +2431,7 @@
         <v>28</v>
       </c>
       <c r="B125">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C125" s="1">
         <v>43427</v>
@@ -2445,7 +2445,7 @@
         <v>28</v>
       </c>
       <c r="B126">
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="C126" s="1">
         <v>43441</v>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="D102">
         <f>schedule!B103</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E102" t="s">
         <v>11</v>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="D103">
         <f>schedule!B104</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -7007,7 +7007,7 @@
       </c>
       <c r="D104">
         <f>schedule!B105</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E104" t="s">
         <v>11</v>
@@ -7040,7 +7040,7 @@
       </c>
       <c r="D105">
         <f>schedule!B106</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E105" t="s">
         <v>11</v>
@@ -7073,7 +7073,7 @@
       </c>
       <c r="D106">
         <f>schedule!B107</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -7106,7 +7106,7 @@
       </c>
       <c r="D107">
         <f>schedule!B108</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E107" t="s">
         <v>11</v>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="D108">
         <f>schedule!B109</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="D109">
         <f>schedule!B110</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E109" t="s">
         <v>11</v>
@@ -7205,7 +7205,7 @@
       </c>
       <c r="D110">
         <f>schedule!B111</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E110" t="s">
         <v>11</v>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="D111">
         <f>schedule!B112</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E111" t="s">
         <v>11</v>
@@ -7271,7 +7271,7 @@
       </c>
       <c r="D112">
         <f>schedule!B113</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E112" t="s">
         <v>11</v>
@@ -7304,7 +7304,7 @@
       </c>
       <c r="D113">
         <f>schedule!B114</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E113" t="s">
         <v>11</v>
@@ -7337,7 +7337,7 @@
       </c>
       <c r="D114">
         <f>schedule!B115</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E114" t="s">
         <v>11</v>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="D115">
         <f>schedule!B116</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E115" t="s">
         <v>11</v>
@@ -7403,7 +7403,7 @@
       </c>
       <c r="D116">
         <f>schedule!B117</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
@@ -7436,7 +7436,7 @@
       </c>
       <c r="D117">
         <f>schedule!B118</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E117" t="s">
         <v>11</v>
@@ -7469,7 +7469,7 @@
       </c>
       <c r="D118">
         <f>schedule!B119</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E118" t="s">
         <v>11</v>
@@ -7502,7 +7502,7 @@
       </c>
       <c r="D119">
         <f>schedule!B120</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E119" t="s">
         <v>11</v>
@@ -7535,7 +7535,7 @@
       </c>
       <c r="D120">
         <f>schedule!B121</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
@@ -7568,7 +7568,7 @@
       </c>
       <c r="D121">
         <f>schedule!B122</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="D122">
         <f>schedule!B123</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E122" t="s">
         <v>11</v>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="D123">
         <f>schedule!B124</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -7667,7 +7667,7 @@
       </c>
       <c r="D124">
         <f>schedule!B125</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E124" t="s">
         <v>11</v>
@@ -7700,7 +7700,7 @@
       </c>
       <c r="D125">
         <f>schedule!B126</f>
-        <v>17543</v>
+        <v>20682</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
@@ -10210,8 +10210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A200"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201:XFD250"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10828,145 +10828,145 @@
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="str">
         <f>sql_raw!A102&amp;sql_raw!B102&amp;sql_raw!C102&amp;sql_raw!D102&amp;sql_raw!E102&amp;TEXT(sql_raw!F102,"yyyy-mm-dd")&amp;sql_raw!G102&amp;TEXT(sql_raw!H102,"yyyy-mm-dd")&amp;sql_raw!I102</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2017-12-15','2018-02-02');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2017-12-15','2018-02-02');</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="str">
         <f>sql_raw!A103&amp;sql_raw!B103&amp;sql_raw!C103&amp;sql_raw!D103&amp;sql_raw!E103&amp;TEXT(sql_raw!F103,"yyyy-mm-dd")&amp;sql_raw!G103&amp;TEXT(sql_raw!H103,"yyyy-mm-dd")&amp;sql_raw!I103</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-01-19','2018-02-16');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-01-19','2018-02-16');</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="str">
         <f>sql_raw!A104&amp;sql_raw!B104&amp;sql_raw!C104&amp;sql_raw!D104&amp;sql_raw!E104&amp;TEXT(sql_raw!F104,"yyyy-mm-dd")&amp;sql_raw!G104&amp;TEXT(sql_raw!H104,"yyyy-mm-dd")&amp;sql_raw!I104</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-02-02','2018-03-02');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-02-02','2018-03-02');</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
         <f>sql_raw!A105&amp;sql_raw!B105&amp;sql_raw!C105&amp;sql_raw!D105&amp;sql_raw!E105&amp;TEXT(sql_raw!F105,"yyyy-mm-dd")&amp;sql_raw!G105&amp;TEXT(sql_raw!H105,"yyyy-mm-dd")&amp;sql_raw!I105</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-02-16','2018-03-16');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-02-16','2018-03-16');</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="str">
         <f>sql_raw!A106&amp;sql_raw!B106&amp;sql_raw!C106&amp;sql_raw!D106&amp;sql_raw!E106&amp;TEXT(sql_raw!F106,"yyyy-mm-dd")&amp;sql_raw!G106&amp;TEXT(sql_raw!H106,"yyyy-mm-dd")&amp;sql_raw!I106</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-03-02','2018-03-30');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-03-02','2018-03-30');</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="str">
         <f>sql_raw!A107&amp;sql_raw!B107&amp;sql_raw!C107&amp;sql_raw!D107&amp;sql_raw!E107&amp;TEXT(sql_raw!F107,"yyyy-mm-dd")&amp;sql_raw!G107&amp;TEXT(sql_raw!H107,"yyyy-mm-dd")&amp;sql_raw!I107</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-03-16','2018-04-13');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-03-16','2018-04-13');</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
         <f>sql_raw!A108&amp;sql_raw!B108&amp;sql_raw!C108&amp;sql_raw!D108&amp;sql_raw!E108&amp;TEXT(sql_raw!F108,"yyyy-mm-dd")&amp;sql_raw!G108&amp;TEXT(sql_raw!H108,"yyyy-mm-dd")&amp;sql_raw!I108</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-03-30','2018-04-27');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-03-30','2018-04-27');</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
         <f>sql_raw!A109&amp;sql_raw!B109&amp;sql_raw!C109&amp;sql_raw!D109&amp;sql_raw!E109&amp;TEXT(sql_raw!F109,"yyyy-mm-dd")&amp;sql_raw!G109&amp;TEXT(sql_raw!H109,"yyyy-mm-dd")&amp;sql_raw!I109</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-04-13','2018-05-11');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-04-13','2018-05-11');</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
         <f>sql_raw!A110&amp;sql_raw!B110&amp;sql_raw!C110&amp;sql_raw!D110&amp;sql_raw!E110&amp;TEXT(sql_raw!F110,"yyyy-mm-dd")&amp;sql_raw!G110&amp;TEXT(sql_raw!H110,"yyyy-mm-dd")&amp;sql_raw!I110</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-04-27','2018-05-25');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-04-27','2018-05-25');</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
         <f>sql_raw!A111&amp;sql_raw!B111&amp;sql_raw!C111&amp;sql_raw!D111&amp;sql_raw!E111&amp;TEXT(sql_raw!F111,"yyyy-mm-dd")&amp;sql_raw!G111&amp;TEXT(sql_raw!H111,"yyyy-mm-dd")&amp;sql_raw!I111</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-05-11','2018-06-08');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-05-11','2018-06-08');</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
         <f>sql_raw!A112&amp;sql_raw!B112&amp;sql_raw!C112&amp;sql_raw!D112&amp;sql_raw!E112&amp;TEXT(sql_raw!F112,"yyyy-mm-dd")&amp;sql_raw!G112&amp;TEXT(sql_raw!H112,"yyyy-mm-dd")&amp;sql_raw!I112</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-05-25','2018-06-22');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-05-25','2018-06-22');</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="str">
         <f>sql_raw!A113&amp;sql_raw!B113&amp;sql_raw!C113&amp;sql_raw!D113&amp;sql_raw!E113&amp;TEXT(sql_raw!F113,"yyyy-mm-dd")&amp;sql_raw!G113&amp;TEXT(sql_raw!H113,"yyyy-mm-dd")&amp;sql_raw!I113</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-06-08','2018-06-20');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-06-08','2018-06-20');</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="str">
         <f>sql_raw!A114&amp;sql_raw!B114&amp;sql_raw!C114&amp;sql_raw!D114&amp;sql_raw!E114&amp;TEXT(sql_raw!F114,"yyyy-mm-dd")&amp;sql_raw!G114&amp;TEXT(sql_raw!H114,"yyyy-mm-dd")&amp;sql_raw!I114</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-06-22','2018-08-03');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-06-22','2018-08-03');</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="str">
         <f>sql_raw!A115&amp;sql_raw!B115&amp;sql_raw!C115&amp;sql_raw!D115&amp;sql_raw!E115&amp;TEXT(sql_raw!F115,"yyyy-mm-dd")&amp;sql_raw!G115&amp;TEXT(sql_raw!H115,"yyyy-mm-dd")&amp;sql_raw!I115</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-06-20','2018-08-17');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-06-20','2018-08-17');</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="str">
         <f>sql_raw!A116&amp;sql_raw!B116&amp;sql_raw!C116&amp;sql_raw!D116&amp;sql_raw!E116&amp;TEXT(sql_raw!F116,"yyyy-mm-dd")&amp;sql_raw!G116&amp;TEXT(sql_raw!H116,"yyyy-mm-dd")&amp;sql_raw!I116</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-08-03','2018-08-31');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-08-03','2018-08-31');</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
         <f>sql_raw!A117&amp;sql_raw!B117&amp;sql_raw!C117&amp;sql_raw!D117&amp;sql_raw!E117&amp;TEXT(sql_raw!F117,"yyyy-mm-dd")&amp;sql_raw!G117&amp;TEXT(sql_raw!H117,"yyyy-mm-dd")&amp;sql_raw!I117</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-08-17','2018-09-14');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-08-17','2018-09-14');</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="str">
         <f>sql_raw!A118&amp;sql_raw!B118&amp;sql_raw!C118&amp;sql_raw!D118&amp;sql_raw!E118&amp;TEXT(sql_raw!F118,"yyyy-mm-dd")&amp;sql_raw!G118&amp;TEXT(sql_raw!H118,"yyyy-mm-dd")&amp;sql_raw!I118</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-08-31','2018-09-28');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-08-31','2018-09-28');</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="str">
         <f>sql_raw!A119&amp;sql_raw!B119&amp;sql_raw!C119&amp;sql_raw!D119&amp;sql_raw!E119&amp;TEXT(sql_raw!F119,"yyyy-mm-dd")&amp;sql_raw!G119&amp;TEXT(sql_raw!H119,"yyyy-mm-dd")&amp;sql_raw!I119</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-09-14','2018-10-12');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-09-14','2018-10-12');</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="str">
         <f>sql_raw!A120&amp;sql_raw!B120&amp;sql_raw!C120&amp;sql_raw!D120&amp;sql_raw!E120&amp;TEXT(sql_raw!F120,"yyyy-mm-dd")&amp;sql_raw!G120&amp;TEXT(sql_raw!H120,"yyyy-mm-dd")&amp;sql_raw!I120</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-09-28','2018-10-26');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-09-28','2018-10-26');</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="str">
         <f>sql_raw!A121&amp;sql_raw!B121&amp;sql_raw!C121&amp;sql_raw!D121&amp;sql_raw!E121&amp;TEXT(sql_raw!F121,"yyyy-mm-dd")&amp;sql_raw!G121&amp;TEXT(sql_raw!H121,"yyyy-mm-dd")&amp;sql_raw!I121</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-10-12','2018-11-09');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-10-12','2018-11-09');</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="str">
         <f>sql_raw!A122&amp;sql_raw!B122&amp;sql_raw!C122&amp;sql_raw!D122&amp;sql_raw!E122&amp;TEXT(sql_raw!F122,"yyyy-mm-dd")&amp;sql_raw!G122&amp;TEXT(sql_raw!H122,"yyyy-mm-dd")&amp;sql_raw!I122</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-10-26','2018-11-23');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-10-26','2018-11-23');</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="str">
         <f>sql_raw!A123&amp;sql_raw!B123&amp;sql_raw!C123&amp;sql_raw!D123&amp;sql_raw!E123&amp;TEXT(sql_raw!F123,"yyyy-mm-dd")&amp;sql_raw!G123&amp;TEXT(sql_raw!H123,"yyyy-mm-dd")&amp;sql_raw!I123</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-11-09','2018-12-07');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-11-09','2018-12-07');</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="str">
         <f>sql_raw!A124&amp;sql_raw!B124&amp;sql_raw!C124&amp;sql_raw!D124&amp;sql_raw!E124&amp;TEXT(sql_raw!F124,"yyyy-mm-dd")&amp;sql_raw!G124&amp;TEXT(sql_raw!H124,"yyyy-mm-dd")&amp;sql_raw!I124</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-11-23','2018-12-21');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-11-23','2018-12-21');</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="str">
         <f>sql_raw!A125&amp;sql_raw!B125&amp;sql_raw!C125&amp;sql_raw!D125&amp;sql_raw!E125&amp;TEXT(sql_raw!F125,"yyyy-mm-dd")&amp;sql_raw!G125&amp;TEXT(sql_raw!H125,"yyyy-mm-dd")&amp;sql_raw!I125</f>
-        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',17543,'2018-12-07','2019-01-25');</v>
+        <v>INSERT INTO sodanca_shipment_schedule (id, supplier_name, supplier_id, cut_off_date, expected_date) VALUES (default, 'Soles - Group 5',20682,'2018-12-07','2019-01-25');</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>